<commit_message>
UPDATE: Added riwayat_thrs table for grouping thrs and informativeness
</commit_message>
<xml_diff>
--- a/Master Keluarga Karyawan Per 25 Apr 2025.xlsx
+++ b/Master Keluarga Karyawan Per 25 Apr 2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\__JOB PROJECT__\__JOB__\RSKI\backend-api-web\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29AA97BA-D2B6-4B57-877C-25E2E49F285A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89940989-FCB2-45CB-8CA3-C8A0D7554EB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7735,10 +7735,10 @@
   <dimension ref="A1:M1365"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C183" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="H3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E65" sqref="E65"/>
+      <selection pane="bottomRight" activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>